<commit_message>
css minifié and html linked to min
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walid/Desktop/Projet 4 - La Panthère/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3C9980-C677-2F4C-89A8-C2EBF9575B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CB241F-A7B3-5D47-B192-F4E6F49A0344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29540" yWindow="-21600" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -326,6 +326,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -540,6 +547,30 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -550,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -559,77 +590,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -850,10 +891,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,10 +1223,10 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="28" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="16" t="s">
@@ -1208,10 +1249,10 @@
       <c r="A15" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="14" t="s">
         <v>58</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -1226,6 +1267,11 @@
       <c r="G15" s="3" t="s">
         <v>53</v>
       </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="31"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>